<commit_message>
Highlighted not complete as red
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint 1 Test Plan.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint 1 Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\Novadapt\XAMPP\htdocs\AC31007\Sprint 1\Sprint_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10720C5-0182-4F87-BD58-B0F86A95F89E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EC63B9-9D42-44C9-B3F1-1415B9161584}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>TESTER COMMENTS</t>
   </si>
@@ -228,6 +228,21 @@
   <si>
     <t>Only responses relevant for a particular question are shown.</t>
   </si>
+  <si>
+    <t>When a questionnaire is submitted, the data is inserted into the database.</t>
+  </si>
+  <si>
+    <t>PK/FK are present, and all fields have a relevant type.</t>
+  </si>
+  <si>
+    <t>Questions in the database match the ones on the questionnaire.</t>
+  </si>
+  <si>
+    <t>Researcher information is stored using a unique ID.</t>
+  </si>
+  <si>
+    <t>Not currently implemented</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +327,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +361,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF40B14B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,7 +452,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -502,6 +523,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -777,15 +801,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -793,15 +817,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,15 +845,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -837,19 +861,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
@@ -861,7 +885,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,7 +893,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,11 +937,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3987,8 +4011,8 @@
   <dimension ref="B1:X71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4297,14 +4321,14 @@
       <c r="E9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="28" t="s">
         <v>62</v>
       </c>
       <c r="J9" s="1"/>
@@ -4453,10 +4477,16 @@
       <c r="E13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="G13" s="15"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="H13" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -4486,10 +4516,16 @@
       <c r="E14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
+      <c r="H14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -4519,10 +4555,16 @@
       <c r="E15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -4552,10 +4594,16 @@
       <c r="E16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="G16" s="15"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="H16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -7330,12 +7378,22 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -7345,22 +7403,27 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>